<commit_message>
relabelled hgv and lgv
</commit_message>
<xml_diff>
--- a/outputs/Fatal_rate_ranges.xlsx
+++ b/outputs/Fatal_rate_ranges.xlsx
@@ -35,10 +35,10 @@
     <t>car/taxi</t>
   </si>
   <si>
-    <t>light goods</t>
-  </si>
-  <si>
-    <t>heavy goods</t>
+    <t>van</t>
+  </si>
+  <si>
+    <t>lorry</t>
   </si>
   <si>
     <t>motorcycle</t>
@@ -121,19 +121,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>3.6930580827843653</v>
+        <v>3.6941528940735493</v>
       </c>
       <c r="C2" t="n">
-        <v>3.1132364554979945</v>
+        <v>3.116195746747314</v>
       </c>
       <c r="D2" t="n">
-        <v>3.9822615706450804</v>
+        <v>3.989104174745653</v>
       </c>
       <c r="E2" t="n">
-        <v>2.3990484560057634</v>
+        <v>2.4034183688700517</v>
       </c>
       <c r="F2" t="n">
-        <v>3.251377749706815</v>
+        <v>3.2547603362365223</v>
       </c>
     </row>
     <row r="3">
@@ -141,19 +141,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0807031368999014</v>
+        <v>3.081163271587731</v>
       </c>
       <c r="C3" t="n">
-        <v>2.456709216024679</v>
+        <v>2.4382992006160045</v>
       </c>
       <c r="D3" t="n">
-        <v>2.8726175804826637</v>
+        <v>2.862070987505259</v>
       </c>
       <c r="E3" t="n">
-        <v>1.9067605082854617</v>
+        <v>1.9119959253232333</v>
       </c>
       <c r="F3" t="n">
-        <v>2.5996010676762453</v>
+        <v>2.5955470064007256</v>
       </c>
     </row>
     <row r="4">
@@ -161,19 +161,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>15.872809891122774</v>
+        <v>15.873055846276467</v>
       </c>
       <c r="C4" t="n">
-        <v>18.789637643705305</v>
+        <v>18.78433824470811</v>
       </c>
       <c r="D4" t="n">
-        <v>19.80793995498357</v>
+        <v>19.77666465776771</v>
       </c>
       <c r="E4" t="n">
-        <v>19.109680746968987</v>
+        <v>19.02291067702824</v>
       </c>
       <c r="F4" t="n">
-        <v>17.117285263672972</v>
+        <v>17.10531817759326</v>
       </c>
     </row>
     <row r="5">
@@ -181,19 +181,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>9.237833016629835</v>
+        <v>9.236023440704061</v>
       </c>
       <c r="C5" t="n">
-        <v>11.492970706996003</v>
+        <v>11.574977021548094</v>
       </c>
       <c r="D5" t="n">
-        <v>8.169109165967425</v>
+        <v>8.257702563934133</v>
       </c>
       <c r="E5" t="n">
-        <v>4.155151798816762</v>
+        <v>4.101707673923155</v>
       </c>
       <c r="F5" t="n">
-        <v>7.676044924202567</v>
+        <v>7.689525045009852</v>
       </c>
     </row>
     <row r="6">
@@ -201,19 +201,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>22.773885176497146</v>
+        <v>22.830163553082294</v>
       </c>
       <c r="C6" t="n">
-        <v>25.26764887833748</v>
+        <v>25.315402881694617</v>
       </c>
       <c r="D6" t="n">
-        <v>18.74813040189869</v>
+        <v>18.783759866192973</v>
       </c>
       <c r="E6" t="n">
-        <v>13.526295826380085</v>
+        <v>13.545189985488175</v>
       </c>
       <c r="F6" t="n">
-        <v>19.22459291610181</v>
+        <v>19.260592274824077</v>
       </c>
     </row>
     <row r="7">
@@ -221,19 +221,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>5.18598869775402</v>
+        <v>5.086910163266265</v>
       </c>
       <c r="C7" t="n">
-        <v>2.0735635853072907</v>
+        <v>2.0854692494558797</v>
       </c>
       <c r="D7" t="n">
-        <v>1.2986418972769274</v>
+        <v>1.3080194394595497</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6371221496634148</v>
+        <v>0.6405785004784111</v>
       </c>
       <c r="F7" t="n">
-        <v>1.131504170633609</v>
+        <v>1.1342981864809742</v>
       </c>
     </row>
   </sheetData>
@@ -272,19 +272,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>3.6949028488113624</v>
+        <v>3.6937273529915524</v>
       </c>
       <c r="C2" t="n">
-        <v>3.112543686569481</v>
+        <v>3.116246408791473</v>
       </c>
       <c r="D2" t="n">
-        <v>3.9801232236815665</v>
+        <v>3.992409031793118</v>
       </c>
       <c r="E2" t="n">
-        <v>2.397047905066885</v>
+        <v>2.4030744172215437</v>
       </c>
       <c r="F2" t="n">
-        <v>3.2513174374389093</v>
+        <v>3.254222463621489</v>
       </c>
     </row>
     <row r="3">
@@ -292,19 +292,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0805572502823155</v>
+        <v>3.083886547937352</v>
       </c>
       <c r="C3" t="n">
-        <v>2.453287608907778</v>
+        <v>2.440970871682321</v>
       </c>
       <c r="D3" t="n">
-        <v>2.866219484904035</v>
+        <v>2.8551700803774684</v>
       </c>
       <c r="E3" t="n">
-        <v>1.9022884558086797</v>
+        <v>1.9091716431730297</v>
       </c>
       <c r="F3" t="n">
-        <v>2.5987721553702166</v>
+        <v>2.592433958499204</v>
       </c>
     </row>
     <row r="4">
@@ -312,19 +312,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>15.883661144831256</v>
+        <v>15.868064863422077</v>
       </c>
       <c r="C4" t="n">
-        <v>18.756406865975027</v>
+        <v>18.76640492276497</v>
       </c>
       <c r="D4" t="n">
-        <v>19.810294697590663</v>
+        <v>19.737857515596275</v>
       </c>
       <c r="E4" t="n">
-        <v>19.11393473460714</v>
+        <v>18.998366123902084</v>
       </c>
       <c r="F4" t="n">
-        <v>17.11391334192286</v>
+        <v>17.107164662443154</v>
       </c>
     </row>
     <row r="5">
@@ -332,19 +332,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>9.168386497921638</v>
+        <v>9.17800066884514</v>
       </c>
       <c r="C5" t="n">
-        <v>11.448229551669534</v>
+        <v>11.535931985043705</v>
       </c>
       <c r="D5" t="n">
-        <v>8.06864490611688</v>
+        <v>8.210616933313968</v>
       </c>
       <c r="E5" t="n">
-        <v>4.123272763419136</v>
+        <v>4.081454768948477</v>
       </c>
       <c r="F5" t="n">
-        <v>7.671795685328905</v>
+        <v>7.687759895905983</v>
       </c>
     </row>
     <row r="6">
@@ -352,19 +352,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>22.707138280899894</v>
+        <v>22.710845304995324</v>
       </c>
       <c r="C6" t="n">
-        <v>25.226947358188205</v>
+        <v>25.250585783853687</v>
       </c>
       <c r="D6" t="n">
-        <v>18.615950014592535</v>
+        <v>18.68087757318349</v>
       </c>
       <c r="E6" t="n">
-        <v>13.510622103243083</v>
+        <v>13.54356827092101</v>
       </c>
       <c r="F6" t="n">
-        <v>19.222541189066504</v>
+        <v>19.239353402432847</v>
       </c>
     </row>
     <row r="7">
@@ -372,19 +372,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>4.85525708568074</v>
+        <v>4.7358412707244675</v>
       </c>
       <c r="C7" t="n">
-        <v>1.9858416358374376</v>
+        <v>2.0450897995898507</v>
       </c>
       <c r="D7" t="n">
-        <v>1.2570762241695905</v>
+        <v>1.2795972939776212</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6179662030588743</v>
+        <v>0.630545229843144</v>
       </c>
       <c r="F7" t="n">
-        <v>1.1216280720915486</v>
+        <v>1.128329419942393</v>
       </c>
     </row>
   </sheetData>
@@ -423,19 +423,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>3.5880152937204404</v>
+        <v>3.593958656889468</v>
       </c>
       <c r="C2" t="n">
-        <v>2.9995227844013925</v>
+        <v>3.0097367866632094</v>
       </c>
       <c r="D2" t="n">
-        <v>3.8439831262979243</v>
+        <v>3.837162613946804</v>
       </c>
       <c r="E2" t="n">
-        <v>2.3125164320704084</v>
+        <v>2.317900416710358</v>
       </c>
       <c r="F2" t="n">
-        <v>3.1956622101276917</v>
+        <v>3.201686370675815</v>
       </c>
     </row>
     <row r="3">
@@ -443,19 +443,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>2.861912982214327</v>
+        <v>2.856885408002161</v>
       </c>
       <c r="C3" t="n">
-        <v>2.194654383821344</v>
+        <v>2.1909200378455176</v>
       </c>
       <c r="D3" t="n">
-        <v>2.6059270033205335</v>
+        <v>2.6013053831465234</v>
       </c>
       <c r="E3" t="n">
-        <v>1.731820920038734</v>
+        <v>1.723418262259683</v>
       </c>
       <c r="F3" t="n">
-        <v>2.4778885815125262</v>
+        <v>2.4841614689420344</v>
       </c>
     </row>
     <row r="4">
@@ -463,19 +463,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>15.165317118803028</v>
+        <v>15.17074088803298</v>
       </c>
       <c r="C4" t="n">
-        <v>17.480622190247566</v>
+        <v>17.426732598547304</v>
       </c>
       <c r="D4" t="n">
-        <v>17.934523586330318</v>
+        <v>17.904038662690066</v>
       </c>
       <c r="E4" t="n">
-        <v>17.114647779719668</v>
+        <v>16.980688977830454</v>
       </c>
       <c r="F4" t="n">
-        <v>16.56372100984389</v>
+        <v>16.545883161703998</v>
       </c>
     </row>
     <row r="5">
@@ -483,19 +483,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>7.740733943411855</v>
+        <v>7.833564835511852</v>
       </c>
       <c r="C5" t="n">
-        <v>9.85876178300213</v>
+        <v>9.768062738474839</v>
       </c>
       <c r="D5" t="n">
-        <v>6.589992019075882</v>
+        <v>6.608737960317089</v>
       </c>
       <c r="E5" t="n">
-        <v>3.360810275814296</v>
+        <v>3.309934748087556</v>
       </c>
       <c r="F5" t="n">
-        <v>6.97656137206047</v>
+        <v>7.02016497189735</v>
       </c>
     </row>
     <row r="6">
@@ -503,19 +503,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>19.97456049352331</v>
+        <v>20.018245957901065</v>
       </c>
       <c r="C6" t="n">
-        <v>22.95101479131809</v>
+        <v>23.034191865079663</v>
       </c>
       <c r="D6" t="n">
-        <v>15.787735745678338</v>
+        <v>15.631866506366196</v>
       </c>
       <c r="E6" t="n">
-        <v>12.121716240984629</v>
+        <v>12.022685780156541</v>
       </c>
       <c r="F6" t="n">
-        <v>18.055412486522908</v>
+        <v>18.155374890454812</v>
       </c>
     </row>
     <row r="7">
@@ -523,19 +523,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>2.5155589511575847</v>
+        <v>2.4394054483147243</v>
       </c>
       <c r="C7" t="n">
-        <v>1.2580563105443383</v>
+        <v>1.3146331230914994</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7961683827410506</v>
+        <v>0.8058288173212159</v>
       </c>
       <c r="E7" t="n">
-        <v>0.42305275976160917</v>
+        <v>0.4193358606355696</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8669344937391277</v>
+        <v>0.8915037414127244</v>
       </c>
     </row>
   </sheetData>
@@ -574,19 +574,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>3.794128035842154</v>
+        <v>3.801126202605852</v>
       </c>
       <c r="C2" t="n">
-        <v>3.235239382859653</v>
+        <v>3.2335543679234746</v>
       </c>
       <c r="D2" t="n">
-        <v>4.139905262822603</v>
+        <v>4.141486241880108</v>
       </c>
       <c r="E2" t="n">
-        <v>2.498008922952507</v>
+        <v>2.490032227956992</v>
       </c>
       <c r="F2" t="n">
-        <v>3.3040729564087195</v>
+        <v>3.3084263161844074</v>
       </c>
     </row>
     <row r="3">
@@ -594,19 +594,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>3.311648336974035</v>
+        <v>3.2980202643835113</v>
       </c>
       <c r="C3" t="n">
-        <v>2.72262121720321</v>
+        <v>2.700545776023522</v>
       </c>
       <c r="D3" t="n">
-        <v>3.1615470229528264</v>
+        <v>3.1408338873226738</v>
       </c>
       <c r="E3" t="n">
-        <v>2.1059721864358845</v>
+        <v>2.1132693217422336</v>
       </c>
       <c r="F3" t="n">
-        <v>2.7250734816108473</v>
+        <v>2.710011973914286</v>
       </c>
     </row>
     <row r="4">
@@ -614,19 +614,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>16.615754363115183</v>
+        <v>16.569697432350722</v>
       </c>
       <c r="C4" t="n">
-        <v>20.25143399557165</v>
+        <v>20.29357807515842</v>
       </c>
       <c r="D4" t="n">
-        <v>21.764548077076256</v>
+        <v>21.776798180977327</v>
       </c>
       <c r="E4" t="n">
-        <v>21.089625859577144</v>
+        <v>20.987738259530566</v>
       </c>
       <c r="F4" t="n">
-        <v>17.704627234819494</v>
+        <v>17.69597721555329</v>
       </c>
     </row>
     <row r="5">
@@ -634,19 +634,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>10.92362016225016</v>
+        <v>10.85615301409685</v>
       </c>
       <c r="C5" t="n">
-        <v>13.407636144216722</v>
+        <v>13.44612101417834</v>
       </c>
       <c r="D5" t="n">
-        <v>10.02190879878088</v>
+        <v>10.100616934402128</v>
       </c>
       <c r="E5" t="n">
-        <v>5.038000726961706</v>
+        <v>4.97629352569548</v>
       </c>
       <c r="F5" t="n">
-        <v>8.382391458482324</v>
+        <v>8.406592746650333</v>
       </c>
     </row>
     <row r="6">
@@ -654,19 +654,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>25.802299633081436</v>
+        <v>25.78934047249593</v>
       </c>
       <c r="C6" t="n">
-        <v>27.80411887316064</v>
+        <v>27.806236893616507</v>
       </c>
       <c r="D6" t="n">
-        <v>22.234768496128762</v>
+        <v>22.326689047482002</v>
       </c>
       <c r="E6" t="n">
-        <v>15.048662749230845</v>
+        <v>15.127470666100837</v>
       </c>
       <c r="F6" t="n">
-        <v>20.372469484741778</v>
+        <v>20.413120054707615</v>
       </c>
     </row>
     <row r="7">
@@ -674,19 +674,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>8.930721480666</v>
+        <v>8.78428830368854</v>
       </c>
       <c r="C7" t="n">
-        <v>3.135567881992599</v>
+        <v>3.0860266315067113</v>
       </c>
       <c r="D7" t="n">
-        <v>1.9906641118679549</v>
+        <v>1.9342917255887289</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9212576079145371</v>
+        <v>0.8948563599626743</v>
       </c>
       <c r="F7" t="n">
-        <v>1.4260083100061285</v>
+        <v>1.3995784706992287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>